<commit_message>
Changed description @DisplayName of classes
</commit_message>
<xml_diff>
--- a/src/docs/testdocumentation.xlsx
+++ b/src/docs/testdocumentation.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDEAProjects\test-ofismag\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32423E8-86DF-4F1A-83CB-B2FC8780EB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5597BD-E4BA-45B9-B522-73CE102075CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-52380" yWindow="-1950" windowWidth="23235" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52035" yWindow="-1605" windowWidth="23235" windowHeight="12810" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
     <sheet name="Testcases" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Testcases!$A$1:$J$54</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
   <si>
     <t>ID checklist</t>
   </si>
@@ -452,6 +455,16 @@
   </si>
   <si>
     <t>В поле "Пароль" ••••••••••••</t>
+  </si>
+  <si>
+    <t>Поле "Электронная почта" имеет красную границу и сообщение "Пользователь с таким адресом электронной почты уже существует.
+Если вы забыли пароль, попробуйте его восстановить"</t>
+  </si>
+  <si>
+    <t>В поле "Электронная почта"  значение "testuser????@mail.ru"</t>
+  </si>
+  <si>
+    <t>В поле "Электронная почта" ввести значение "testuser????@mail.ru"</t>
   </si>
 </sst>
 </file>
@@ -500,18 +513,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -710,7 +717,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -748,15 +755,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -787,6 +788,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -817,17 +824,38 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -835,65 +863,38 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1475,7 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B28" s="6" t="s">
@@ -1486,7 +1487,7 @@
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="61" t="s">
+      <c r="A29" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -1498,14 +1499,14 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="36" t="s">
         <v>111</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D30" s="4"/>
     </row>
@@ -1521,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE60BC1-EA23-40DD-812C-72C6DCC8A456}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42:J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,77 +1542,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23">
         <f>COUNTA(H3:H307)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="23">
         <f>COUNTA(I3:I307)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="23">
         <f>COUNTA(J3:J307)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="16" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1723,7 +1724,7 @@
       <c r="E8" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>104</v>
       </c>
       <c r="G8" s="10"/>
@@ -1782,639 +1783,880 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="24">
         <v>1</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27" t="s">
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48" t="s">
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="26">
+      <c r="A12" s="54"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="24">
         <v>2</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="26">
+      <c r="A13" s="54"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="24">
         <v>3</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="26">
+      <c r="A14" s="54"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="24">
         <v>4</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="26">
+      <c r="A15" s="55"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="24">
         <v>5</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="26">
         <v>1</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40" t="s">
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="28">
+      <c r="A17" s="57"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="26">
         <v>2</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="28">
+      <c r="A18" s="57"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="26">
         <v>3</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="28">
+      <c r="A19" s="57"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="26">
         <v>4</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>1</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31" t="s">
+      <c r="E20" s="29"/>
+      <c r="F20" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="30">
+      <c r="A21" s="59"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="28">
         <v>2</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="30">
+      <c r="A22" s="59"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="28">
         <v>3</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
     </row>
     <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="30">
+      <c r="A23" s="59"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="28">
         <v>4</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="30">
         <v>1</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33" t="s">
+      <c r="E24" s="31"/>
+      <c r="F24" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38" t="s">
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="32">
+      <c r="A25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="30">
         <v>2</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C26" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="32">
         <v>1</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E26" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55" t="s">
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="34">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="32">
         <v>2</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="34">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="32">
         <v>3</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="34">
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="32">
         <v>4</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="34">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="32">
         <v>5</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="34">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="32">
         <v>6</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="34">
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="32">
         <v>7</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="34">
+      <c r="A33" s="38"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="32">
         <v>8</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="32">
+        <v>9</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+    </row>
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="38"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="32">
+        <v>10</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="38"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="32">
+        <v>11</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+    </row>
+    <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="32">
+        <v>11</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+    </row>
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="32">
+        <v>12</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="34">
+        <v>1</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="41"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="34">
+        <v>2</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="41"/>
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="42"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="34">
+        <v>3</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="32">
+        <v>1</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="32">
+        <v>2</v>
+      </c>
+      <c r="E43" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+    </row>
+    <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="38"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="32">
+        <v>3</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="38"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="32">
+        <v>4</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="38"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="32">
+        <v>5</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="32">
+        <v>6</v>
+      </c>
+      <c r="E47" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="38"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="38"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="38"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="32">
+        <v>7</v>
+      </c>
+      <c r="E48" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="38"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="32">
+        <v>8</v>
+      </c>
+      <c r="E49" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F49" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="G33" s="56"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="34">
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="38"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="38"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="32">
         <v>9</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E50" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F50" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-    </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="34">
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="38"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="32">
         <v>10</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E51" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="35" t="s">
+      <c r="F51" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="56"/>
-    </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="34">
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
+    </row>
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="38"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="32">
         <v>11</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E52" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F52" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-    </row>
-    <row r="37" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="34">
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+    </row>
+    <row r="53" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="38"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="32">
         <v>11</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E53" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F53" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="57"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="34">
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+    </row>
+    <row r="54" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="39"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="32">
         <v>12</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E54" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="F38" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="57"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="58" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="58" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="36">
-        <v>1</v>
-      </c>
-      <c r="E39" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F39" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="36">
-        <v>2</v>
-      </c>
-      <c r="E40" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-    </row>
-    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="60"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="36">
-        <v>3</v>
-      </c>
-      <c r="E41" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" s="60"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
+      <c r="F54" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="49">
+    <mergeCell ref="I42:I54"/>
+    <mergeCell ref="J42:J54"/>
+    <mergeCell ref="A42:A54"/>
+    <mergeCell ref="B42:B54"/>
+    <mergeCell ref="C42:C54"/>
+    <mergeCell ref="G42:G54"/>
+    <mergeCell ref="H42:H54"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="C11:C15"/>
     <mergeCell ref="J26:J38"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="B39:B41"/>
@@ -2429,34 +2671,6 @@
     <mergeCell ref="G26:G38"/>
     <mergeCell ref="H26:H38"/>
     <mergeCell ref="I26:I38"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="J11:J15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>